<commit_message>
Finished running two tests for both single classification and group classification. Now just have to run them with newrb, start the report, and possibly run a few more tests
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Single Classification" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="30">
   <si>
     <t>Rede</t>
   </si>
@@ -120,6 +120,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -179,12 +180,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -207,8 +212,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2792,20 +2797,2574 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="19.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.1071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.9438775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0.99996</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0.58939</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>252140</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>418</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0.83471</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0.34344</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>351</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>210460</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>41674</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>671</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.48224</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0.30596</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>313</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>121610</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>130570</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>710</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0.99989</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0.58944</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>603</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>252080</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>420</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0.71533</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0.93157</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>953</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>180390</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>71787</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0.79702</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0.49365</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>505</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>200990</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>51188</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>518</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0.99071</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0.29717</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>304</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>249840</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>2342</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>719</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>252180</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>1023</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0.97408</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0.74052</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>12478</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>332</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>219</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>239550</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0.99997</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0.64809</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>663</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>252170</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>360</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0.97967</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.56706</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>482</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>13832</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>287</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>368</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>238230</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0.99963</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>143160</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>986</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>109000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0.9899</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0.79374</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>812</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>249630</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>2548</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>211</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>0.92567</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0.88172</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>902</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>233440</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>18745</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>0.98036</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0.84164</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>861</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>247230</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>4953</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>162</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0.99022</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0.7598</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>775</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>243400</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>2404</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>245</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>6380</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0.99892</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0.85239</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>872</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>251910</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>273</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>151</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0.99209</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0.8348</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>854</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>250180</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>1995</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>1023</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>252180</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>252180</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>1020</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>1023</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>252180</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>252180</v>
+      </c>
+      <c r="K24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>1023</v>
+      </c>
+      <c r="M24" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="n">
+        <v>253170</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>0.96717</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0.45455</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>465</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>243900</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>8280</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>558</v>
+      </c>
+      <c r="M26" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>0.51044</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0.95797</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>980</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>128720</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>123460</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="M27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0.69697</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>713</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>248400</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>3782</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>310</v>
+      </c>
+      <c r="M28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>1023</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>252180</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0.74658</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0.22483</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>188270</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>63907</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>793</v>
+      </c>
+      <c r="M30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>0.99833</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>0.83871</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>858</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>251760</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>421</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>165</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>0.99301</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0.84457</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>864</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>250420</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>1763</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>159</v>
+      </c>
+      <c r="M32" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>0.14208</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>0.83933</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>653</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>6244</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>37703</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="M34" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>0.019683</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>0.9313</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>732</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>865</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>43082</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="M35" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>0.093772</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>0.90712</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>713</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>4121</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>39826</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="M36" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>0.99993</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>0.32398</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>254</v>
+      </c>
+      <c r="J37" s="2" t="n">
+        <v>42512</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L37" s="2" t="n">
+        <v>530</v>
+      </c>
+      <c r="M37" s="2" t="n">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>0.9103</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>0.60305</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>474</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>40005</v>
+      </c>
+      <c r="K38" s="2" t="n">
+        <v>3942</v>
+      </c>
+      <c r="L38" s="2" t="n">
+        <v>312</v>
+      </c>
+      <c r="M38" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>0.092043</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>0.90712</v>
+      </c>
+      <c r="I39" s="2" t="n">
+        <v>713</v>
+      </c>
+      <c r="J39" s="2" t="n">
+        <v>4045</v>
+      </c>
+      <c r="K39" s="2" t="n">
+        <v>39902</v>
+      </c>
+      <c r="L39" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="M39" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>0.95772</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0.11196</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>42089</v>
+      </c>
+      <c r="K40" s="2" t="n">
+        <v>1858</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>698</v>
+      </c>
+      <c r="M40" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="M41" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>557</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="M42" s="2" t="n">
+        <v>44095</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>0.99993</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>0.30025</v>
+      </c>
+      <c r="I43" s="2" t="n">
+        <v>236</v>
+      </c>
+      <c r="J43" s="2" t="n">
+        <v>43944</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <v>550</v>
+      </c>
+      <c r="M43" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>0.94877</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="J44" s="2" t="n">
+        <v>8185</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>442</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>168</v>
+      </c>
+      <c r="M44" s="2" t="n">
+        <v>35882</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>0.0065147</v>
+      </c>
+      <c r="I45" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J45" s="2" t="n">
+        <v>6439</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <v>305</v>
+      </c>
+      <c r="M45" s="2" t="n">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>0.34291</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0.86641</v>
+      </c>
+      <c r="I46" s="2" t="n">
+        <v>681</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>15070</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>28877</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="M46" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <v>0.9002</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0.70625</v>
+      </c>
+      <c r="I47" s="2" t="n">
+        <v>452</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>26565</v>
+      </c>
+      <c r="K47" s="2" t="n">
+        <v>2945</v>
+      </c>
+      <c r="L47" s="2" t="n">
+        <v>188</v>
+      </c>
+      <c r="M47" s="2" t="n">
+        <v>14583</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G48" s="2" t="n">
+        <v>0.94748</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>0.23028</v>
+      </c>
+      <c r="I48" s="2" t="n">
+        <v>181</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>41639</v>
+      </c>
+      <c r="K48" s="2" t="n">
+        <v>2308</v>
+      </c>
+      <c r="L48" s="2" t="n">
+        <v>605</v>
+      </c>
+      <c r="M48" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G49" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>0.081841</v>
+      </c>
+      <c r="I49" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>12146</v>
+      </c>
+      <c r="K49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2" t="n">
+        <v>359</v>
+      </c>
+      <c r="M49" s="2" t="n">
+        <v>32196</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>0.21992</v>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>0.89695</v>
+      </c>
+      <c r="I50" s="2" t="n">
+        <v>705</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>9665</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>34282</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="M50" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0.94441</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0.55725</v>
+      </c>
+      <c r="I51" s="2" t="n">
+        <v>438</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>41504</v>
+      </c>
+      <c r="K51" s="2" t="n">
+        <v>2443</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>348</v>
+      </c>
+      <c r="M51" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="J52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G53" s="2" t="n">
+        <v>0.99993</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <v>43944</v>
+      </c>
+      <c r="K53" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="M53" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="L54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G55" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2" t="n">
+        <v>43947</v>
+      </c>
+      <c r="K55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="M55" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>274</v>
+      </c>
+      <c r="K56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2" t="n">
+        <v>44459</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0.99997</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>0.37054</v>
+      </c>
+      <c r="I57" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>35103</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L57" s="2" t="n">
+        <v>423</v>
+      </c>
+      <c r="M57" s="2" t="n">
+        <v>8957</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>0.88868</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>0.50254</v>
+      </c>
+      <c r="I58" s="2" t="n">
+        <v>395</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>39055</v>
+      </c>
+      <c r="K58" s="2" t="n">
+        <v>4892</v>
+      </c>
+      <c r="L58" s="2" t="n">
+        <v>391</v>
+      </c>
+      <c r="M58" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>0.98751</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>0.51145</v>
+      </c>
+      <c r="I59" s="2" t="n">
+        <v>402</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>43398</v>
+      </c>
+      <c r="K59" s="2" t="n">
+        <v>549</v>
+      </c>
+      <c r="L59" s="2" t="n">
+        <v>384</v>
+      </c>
+      <c r="M59" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>4.5509E-005</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2" t="n">
+        <v>786</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K60" s="2" t="n">
+        <v>43945</v>
+      </c>
+      <c r="L60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>0.10165</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>0.79771</v>
+      </c>
+      <c r="I61" s="2" t="n">
+        <v>627</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <v>4467</v>
+      </c>
+      <c r="K61" s="2" t="n">
+        <v>39480</v>
+      </c>
+      <c r="L61" s="2" t="n">
+        <v>159</v>
+      </c>
+      <c r="M61" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>0.99315</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>0.58779</v>
+      </c>
+      <c r="I62" s="2" t="n">
+        <v>462</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <v>43646</v>
+      </c>
+      <c r="K62" s="2" t="n">
+        <v>301</v>
+      </c>
+      <c r="L62" s="2" t="n">
+        <v>324</v>
+      </c>
+      <c r="M62" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>0.983</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>0.58906</v>
+      </c>
+      <c r="I63" s="2" t="n">
+        <v>463</v>
+      </c>
+      <c r="J63" s="2" t="n">
+        <v>43200</v>
+      </c>
+      <c r="K63" s="2" t="n">
+        <v>747</v>
+      </c>
+      <c r="L63" s="2" t="n">
+        <v>323</v>
+      </c>
+      <c r="M63" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated test results and started writing the report
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -2799,8 +2799,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2880,6 +2880,27 @@
       <c r="F2" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="G2" s="2" t="n">
+        <v>0.90435</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0.89412</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>912</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>228070</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>24123</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
Single classifications tests are done!
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="32">
   <si>
     <t>Rede</t>
   </si>
@@ -223,8 +223,8 @@
   </sheetPr>
   <dimension ref="A1:M187"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G126" activeCellId="0" sqref="G126:M156"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G157" activeCellId="0" sqref="G157:M187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6660,6 +6660,27 @@
       <c r="F157" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G157" s="2" t="n">
+        <v>0.90908</v>
+      </c>
+      <c r="H157" s="2" t="n">
+        <v>0.68407</v>
+      </c>
+      <c r="I157" s="2" t="n">
+        <v>747</v>
+      </c>
+      <c r="J157" s="2" t="n">
+        <v>103280</v>
+      </c>
+      <c r="K157" s="2" t="n">
+        <v>10330</v>
+      </c>
+      <c r="L157" s="2" t="n">
+        <v>345</v>
+      </c>
+      <c r="M157" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
@@ -6680,6 +6701,27 @@
       <c r="F158" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G158" s="2" t="n">
+        <v>0.17118</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>0.78733</v>
+      </c>
+      <c r="I158" s="2" t="n">
+        <v>733</v>
+      </c>
+      <c r="J158" s="2" t="n">
+        <v>18273</v>
+      </c>
+      <c r="K158" s="2" t="n">
+        <v>88474</v>
+      </c>
+      <c r="L158" s="2" t="n">
+        <v>198</v>
+      </c>
+      <c r="M158" s="2" t="n">
+        <v>7026</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
@@ -6700,6 +6742,27 @@
       <c r="F159" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G159" s="2" t="n">
+        <v>0.094781</v>
+      </c>
+      <c r="H159" s="2" t="n">
+        <v>0.90221</v>
+      </c>
+      <c r="I159" s="2" t="n">
+        <v>941</v>
+      </c>
+      <c r="J159" s="2" t="n">
+        <v>10438</v>
+      </c>
+      <c r="K159" s="2" t="n">
+        <v>99689</v>
+      </c>
+      <c r="L159" s="2" t="n">
+        <v>102</v>
+      </c>
+      <c r="M159" s="2" t="n">
+        <v>3534</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
@@ -6720,6 +6783,27 @@
       <c r="F160" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G160" s="2" t="n">
+        <v>0.12901</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>0.80971</v>
+      </c>
+      <c r="I160" s="2" t="n">
+        <v>851</v>
+      </c>
+      <c r="J160" s="2" t="n">
+        <v>14477</v>
+      </c>
+      <c r="K160" s="2" t="n">
+        <v>97739</v>
+      </c>
+      <c r="L160" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="M160" s="2" t="n">
+        <v>1437</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
@@ -6740,6 +6824,27 @@
       <c r="F161" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G161" s="2" t="n">
+        <v>0.95848</v>
+      </c>
+      <c r="H161" s="2" t="n">
+        <v>0.44645</v>
+      </c>
+      <c r="I161" s="2" t="n">
+        <v>371</v>
+      </c>
+      <c r="J161" s="2" t="n">
+        <v>61825</v>
+      </c>
+      <c r="K161" s="2" t="n">
+        <v>2678</v>
+      </c>
+      <c r="L161" s="2" t="n">
+        <v>460</v>
+      </c>
+      <c r="M161" s="2" t="n">
+        <v>49370</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
@@ -6760,6 +6865,27 @@
       <c r="F162" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G162" s="2" t="n">
+        <v>0.83257</v>
+      </c>
+      <c r="H162" s="2" t="n">
+        <v>0.68541</v>
+      </c>
+      <c r="I162" s="2" t="n">
+        <v>719</v>
+      </c>
+      <c r="J162" s="2" t="n">
+        <v>84592</v>
+      </c>
+      <c r="K162" s="2" t="n">
+        <v>17011</v>
+      </c>
+      <c r="L162" s="2" t="n">
+        <v>330</v>
+      </c>
+      <c r="M162" s="2" t="n">
+        <v>12052</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
@@ -6780,6 +6906,27 @@
       <c r="F163" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G163" s="2" t="n">
+        <v>0.12469</v>
+      </c>
+      <c r="H163" s="2" t="n">
+        <v>0.79412</v>
+      </c>
+      <c r="I163" s="2" t="n">
+        <v>810</v>
+      </c>
+      <c r="J163" s="2" t="n">
+        <v>13924</v>
+      </c>
+      <c r="K163" s="2" t="n">
+        <v>97745</v>
+      </c>
+      <c r="L163" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="M163" s="2" t="n">
+        <v>2015</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
@@ -6800,6 +6947,27 @@
       <c r="F164" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G164" s="2" t="n">
+        <v>0.9353</v>
+      </c>
+      <c r="H164" s="2" t="n">
+        <v>0.1902</v>
+      </c>
+      <c r="I164" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="J164" s="2" t="n">
+        <v>104660</v>
+      </c>
+      <c r="K164" s="2" t="n">
+        <v>7240</v>
+      </c>
+      <c r="L164" s="2" t="n">
+        <v>826</v>
+      </c>
+      <c r="M164" s="2" t="n">
+        <v>1782</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
@@ -6820,6 +6988,27 @@
       <c r="F165" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G165" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J165" s="2" t="n">
+        <v>112000</v>
+      </c>
+      <c r="K165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L165" s="2" t="n">
+        <v>1047</v>
+      </c>
+      <c r="M165" s="2" t="n">
+        <v>1659</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
@@ -6840,6 +7029,27 @@
       <c r="F166" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G166" s="2" t="n">
+        <v>0.87379</v>
+      </c>
+      <c r="H166" s="2" t="n">
+        <v>0.11864</v>
+      </c>
+      <c r="I166" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J166" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="K166" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L166" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="M166" s="2" t="n">
+        <v>114540</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
@@ -6860,6 +7070,27 @@
       <c r="F167" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G167" s="2" t="n">
+        <v>0.99036</v>
+      </c>
+      <c r="H167" s="2" t="n">
+        <v>0.3283</v>
+      </c>
+      <c r="I167" s="2" t="n">
+        <v>348</v>
+      </c>
+      <c r="J167" s="2" t="n">
+        <v>110600</v>
+      </c>
+      <c r="K167" s="2" t="n">
+        <v>1077</v>
+      </c>
+      <c r="L167" s="2" t="n">
+        <v>712</v>
+      </c>
+      <c r="M167" s="2" t="n">
+        <v>1971</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
@@ -6880,6 +7111,27 @@
       <c r="F168" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G168" s="2" t="n">
+        <v>0.27578</v>
+      </c>
+      <c r="H168" s="2" t="n">
+        <v>0.62245</v>
+      </c>
+      <c r="I168" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="J168" s="2" t="n">
+        <v>1230</v>
+      </c>
+      <c r="K168" s="2" t="n">
+        <v>3230</v>
+      </c>
+      <c r="L168" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="M168" s="2" t="n">
+        <v>110050</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
@@ -6900,6 +7152,27 @@
       <c r="F169" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G169" s="2" t="n">
+        <v>0.43457</v>
+      </c>
+      <c r="H169" s="2" t="n">
+        <v>0.51316</v>
+      </c>
+      <c r="I169" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="J169" s="2" t="n">
+        <v>870</v>
+      </c>
+      <c r="K169" s="2" t="n">
+        <v>1132</v>
+      </c>
+      <c r="L169" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="M169" s="2" t="n">
+        <v>112630</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
@@ -6920,6 +7193,27 @@
       <c r="F170" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G170" s="2" t="n">
+        <v>0.39432</v>
+      </c>
+      <c r="H170" s="2" t="n">
+        <v>0.79468</v>
+      </c>
+      <c r="I170" s="2" t="n">
+        <v>836</v>
+      </c>
+      <c r="J170" s="2" t="n">
+        <v>42894</v>
+      </c>
+      <c r="K170" s="2" t="n">
+        <v>65886</v>
+      </c>
+      <c r="L170" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="M170" s="2" t="n">
+        <v>4872</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
@@ -6940,6 +7234,27 @@
       <c r="F171" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G171" s="2" t="n">
+        <v>0.39054</v>
+      </c>
+      <c r="H171" s="2" t="n">
+        <v>0.71003</v>
+      </c>
+      <c r="I171" s="2" t="n">
+        <v>524</v>
+      </c>
+      <c r="J171" s="2" t="n">
+        <v>12304</v>
+      </c>
+      <c r="K171" s="2" t="n">
+        <v>19201</v>
+      </c>
+      <c r="L171" s="2" t="n">
+        <v>214</v>
+      </c>
+      <c r="M171" s="2" t="n">
+        <v>82461</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
@@ -6960,6 +7275,27 @@
       <c r="F172" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G172" s="2" t="n">
+        <v>0.91155</v>
+      </c>
+      <c r="H172" s="2" t="n">
+        <v>0.32202</v>
+      </c>
+      <c r="I172" s="2" t="n">
+        <v>351</v>
+      </c>
+      <c r="J172" s="2" t="n">
+        <v>103520</v>
+      </c>
+      <c r="K172" s="2" t="n">
+        <v>10044</v>
+      </c>
+      <c r="L172" s="2" t="n">
+        <v>739</v>
+      </c>
+      <c r="M172" s="2" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
@@ -6980,6 +7316,27 @@
       <c r="F173" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G173" s="2" t="n">
+        <v>0.96949</v>
+      </c>
+      <c r="H173" s="2" t="n">
+        <v>0.71429</v>
+      </c>
+      <c r="I173" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J173" s="2" t="n">
+        <v>4926</v>
+      </c>
+      <c r="K173" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="L173" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="M173" s="2" t="n">
+        <v>109480</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
@@ -7000,6 +7357,27 @@
       <c r="F174" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G174" s="2" t="n">
+        <v>0.32022</v>
+      </c>
+      <c r="H174" s="2" t="n">
+        <v>0.81985</v>
+      </c>
+      <c r="I174" s="2" t="n">
+        <v>892</v>
+      </c>
+      <c r="J174" s="2" t="n">
+        <v>36322</v>
+      </c>
+      <c r="K174" s="2" t="n">
+        <v>77107</v>
+      </c>
+      <c r="L174" s="2" t="n">
+        <v>196</v>
+      </c>
+      <c r="M174" s="2" t="n">
+        <v>187</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
@@ -7020,6 +7398,27 @@
       <c r="F175" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G175" s="2" t="n">
+        <v>0.92473</v>
+      </c>
+      <c r="H175" s="2" t="n">
+        <v>0.65161</v>
+      </c>
+      <c r="I175" s="2" t="n">
+        <v>707</v>
+      </c>
+      <c r="J175" s="2" t="n">
+        <v>104650</v>
+      </c>
+      <c r="K175" s="2" t="n">
+        <v>8519</v>
+      </c>
+      <c r="L175" s="2" t="n">
+        <v>378</v>
+      </c>
+      <c r="M175" s="2" t="n">
+        <v>447</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
@@ -7040,6 +7439,27 @@
       <c r="F176" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G176" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H176" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I176" s="2" t="n">
+        <v>1091</v>
+      </c>
+      <c r="J176" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K176" s="2" t="n">
+        <v>113090</v>
+      </c>
+      <c r="L176" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M176" s="2" t="n">
+        <v>526</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
@@ -7060,6 +7480,27 @@
       <c r="F177" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G177" s="2" t="n">
+        <v>0.99908</v>
+      </c>
+      <c r="H177" s="2" t="n">
+        <v>0.00091996</v>
+      </c>
+      <c r="I177" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J177" s="2" t="n">
+        <v>112470</v>
+      </c>
+      <c r="K177" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="L177" s="2" t="n">
+        <v>1086</v>
+      </c>
+      <c r="M177" s="2" t="n">
+        <v>1040</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
@@ -7080,6 +7521,27 @@
       <c r="F178" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H178" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I178" s="2" t="n">
+        <v>1091</v>
+      </c>
+      <c r="J178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K178" s="2" t="n">
+        <v>113340</v>
+      </c>
+      <c r="L178" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M178" s="2" t="n">
+        <v>275</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
@@ -7100,6 +7562,27 @@
       <c r="F179" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G179" s="2" t="n">
+        <v>0.99987</v>
+      </c>
+      <c r="H179" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I179" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J179" s="2" t="n">
+        <v>112700</v>
+      </c>
+      <c r="K179" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="L179" s="2" t="n">
+        <v>1087</v>
+      </c>
+      <c r="M179" s="2" t="n">
+        <v>907</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
@@ -7120,6 +7603,27 @@
       <c r="F180" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G180" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I180" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J180" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K180" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="L180" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M180" s="2" t="n">
+        <v>114650</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
@@ -7140,6 +7644,27 @@
       <c r="F181" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G181" s="2" t="n">
+        <v>0.97746</v>
+      </c>
+      <c r="H181" s="2" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="I181" s="2" t="n">
+        <v>309</v>
+      </c>
+      <c r="J181" s="2" t="n">
+        <v>43807</v>
+      </c>
+      <c r="K181" s="2" t="n">
+        <v>1010</v>
+      </c>
+      <c r="L181" s="2" t="n">
+        <v>432</v>
+      </c>
+      <c r="M181" s="2" t="n">
+        <v>69146</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
@@ -7160,6 +7685,27 @@
       <c r="F182" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G182" s="2" t="n">
+        <v>0.88178</v>
+      </c>
+      <c r="H182" s="2" t="n">
+        <v>0.56792</v>
+      </c>
+      <c r="I182" s="2" t="n">
+        <v>602</v>
+      </c>
+      <c r="J182" s="2" t="n">
+        <v>99930</v>
+      </c>
+      <c r="K182" s="2" t="n">
+        <v>13398</v>
+      </c>
+      <c r="L182" s="2" t="n">
+        <v>458</v>
+      </c>
+      <c r="M182" s="2" t="n">
+        <v>316</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
@@ -7180,6 +7726,27 @@
       <c r="F183" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G183" s="2" t="n">
+        <v>0.93928</v>
+      </c>
+      <c r="H183" s="2" t="n">
+        <v>0.59961</v>
+      </c>
+      <c r="I183" s="2" t="n">
+        <v>614</v>
+      </c>
+      <c r="J183" s="2" t="n">
+        <v>105170</v>
+      </c>
+      <c r="K183" s="2" t="n">
+        <v>6799</v>
+      </c>
+      <c r="L183" s="2" t="n">
+        <v>410</v>
+      </c>
+      <c r="M183" s="2" t="n">
+        <v>1708</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
@@ -7200,6 +7767,27 @@
       <c r="F184" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G184" s="2" t="n">
+        <v>0.0003363</v>
+      </c>
+      <c r="H184" s="2" t="n">
+        <v>0.99908</v>
+      </c>
+      <c r="I184" s="2" t="n">
+        <v>1090</v>
+      </c>
+      <c r="J184" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="K184" s="2" t="n">
+        <v>112960</v>
+      </c>
+      <c r="L184" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M184" s="2" t="n">
+        <v>618</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
@@ -7220,6 +7808,27 @@
       <c r="F185" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G185" s="2" t="n">
+        <v>0.14145</v>
+      </c>
+      <c r="H185" s="2" t="n">
+        <v>0.68816</v>
+      </c>
+      <c r="I185" s="2" t="n">
+        <v>715</v>
+      </c>
+      <c r="J185" s="2" t="n">
+        <v>15871</v>
+      </c>
+      <c r="K185" s="2" t="n">
+        <v>96330</v>
+      </c>
+      <c r="L185" s="2" t="n">
+        <v>324</v>
+      </c>
+      <c r="M185" s="2" t="n">
+        <v>1464</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
@@ -7240,6 +7849,27 @@
       <c r="F186" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="G186" s="2" t="n">
+        <v>0.95605</v>
+      </c>
+      <c r="H186" s="2" t="n">
+        <v>0.63477</v>
+      </c>
+      <c r="I186" s="2" t="n">
+        <v>690</v>
+      </c>
+      <c r="J186" s="2" t="n">
+        <v>108380</v>
+      </c>
+      <c r="K186" s="2" t="n">
+        <v>4982</v>
+      </c>
+      <c r="L186" s="2" t="n">
+        <v>397</v>
+      </c>
+      <c r="M186" s="2" t="n">
+        <v>253</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
@@ -7259,6 +7889,27 @@
       </c>
       <c r="F187" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="G187" s="2" t="n">
+        <v>0.94371</v>
+      </c>
+      <c r="H187" s="2" t="n">
+        <v>0.66269</v>
+      </c>
+      <c r="I187" s="2" t="n">
+        <v>723</v>
+      </c>
+      <c r="J187" s="2" t="n">
+        <v>106990</v>
+      </c>
+      <c r="K187" s="2" t="n">
+        <v>6382</v>
+      </c>
+      <c r="L187" s="2" t="n">
+        <v>368</v>
+      </c>
+      <c r="M187" s="2" t="n">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -7280,7 +7931,7 @@
   <dimension ref="A1:M187"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A126" activeCellId="1" sqref="G126:M156 A126"/>
+      <selection pane="topLeft" activeCell="A126" activeCellId="1" sqref="G157:M187 A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Updates on the results
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="215" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="215" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Single Classification" sheetId="1" state="visible" r:id="rId2"/>
@@ -239,8 +239,8 @@
   </sheetPr>
   <dimension ref="A1:N218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188:N188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8512,6 +8512,27 @@
       <c r="G188" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="H188" s="2" t="n">
+        <v>0.66287</v>
+      </c>
+      <c r="I188" s="2" t="n">
+        <v>0.70339</v>
+      </c>
+      <c r="J188" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="K188" s="2" t="n">
+        <v>82466</v>
+      </c>
+      <c r="L188" s="2" t="n">
+        <v>41941</v>
+      </c>
+      <c r="M188" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="N188" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
@@ -9851,8 +9872,8 @@
   </sheetPr>
   <dimension ref="A1:N218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188:N188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -18123,6 +18144,27 @@
       <c r="G188" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="H188" s="2" t="n">
+        <v>0.74893</v>
+      </c>
+      <c r="I188" s="2" t="n">
+        <v>0.86992</v>
+      </c>
+      <c r="J188" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="K188" s="2" t="n">
+        <v>93161</v>
+      </c>
+      <c r="L188" s="2" t="n">
+        <v>31231</v>
+      </c>
+      <c r="M188" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N188" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
@@ -19463,7 +19505,7 @@
   <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+      <selection pane="topLeft" activeCell="E45" activeCellId="1" sqref="H188:N188 E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -23779,8 +23821,8 @@
   </sheetPr>
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="H188:N188 K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Talked about the results in the report: The only thing missing is the dimensionality reduction and the conclusions
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="215" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Single Classification" sheetId="1" state="visible" r:id="rId2"/>
@@ -239,8 +239,8 @@
   </sheetPr>
   <dimension ref="A1:N218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188:N188"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188:H208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9857,7 +9857,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9872,8 +9872,8 @@
   </sheetPr>
   <dimension ref="A1:N218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H188" activeCellId="0" sqref="H188:N188"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -19489,7 +19489,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -19504,8 +19504,8 @@
   </sheetPr>
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="1" sqref="H188:N188 E45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -23806,7 +23806,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -23821,8 +23821,8 @@
   </sheetPr>
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="1" sqref="H188:N188 K5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -28123,7 +28123,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Corrected bug in the feature selection code. Started reformulating the report and updating the images to the last versions of the results and the application's gui
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -223,27 +223,27 @@
   </sheetPr>
   <dimension ref="A1:O559"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A373" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C394" activeCellId="1" sqref="I374:O466 C394"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="1" sqref="O:O H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.6530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.1581632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
@@ -26538,27 +26538,27 @@
   </sheetPr>
   <dimension ref="A1:O559"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A367" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I374" activeCellId="0" sqref="I374:O466"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O:O"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3265306122449"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3571428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.6530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.1581632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Updated tests in the report. Added script where we will train all the networks for the correlation tests
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="224" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="224" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Single Classification" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Group Classification" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Reduced Dimension Single" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Reduced Dimension Group" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -223,8 +225,8 @@
   </sheetPr>
   <dimension ref="A1:O559"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="1" sqref="O:O H20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J94" activeCellId="0" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26523,7 +26525,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -26538,8 +26540,8 @@
   </sheetPr>
   <dimension ref="A1:O559"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O:O"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -52838,6 +52840,58 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>

</xml_diff>

<commit_message>
Finished the description of the second round of tests. Missing: Conclusions and Attachments
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -233,7 +233,7 @@
   <dimension ref="A1:O559"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="J2:P109 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26548,7 +26548,7 @@
   <dimension ref="A1:O559"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="1" sqref="J2:P109 B43"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -52862,8 +52862,8 @@
   </sheetPr>
   <dimension ref="A1:R217"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B128" activeCellId="1" sqref="J2:P109 B128"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -52886,13 +52886,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -63758,7 +63758,7 @@
   <dimension ref="A1:P217"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:P109"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -63782,13 +63782,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">

</xml_diff>

<commit_message>
Finished first version of the report!
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -233,7 +233,7 @@
   <dimension ref="A1:O559"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26532,7 +26532,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -52847,7 +52847,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -63742,7 +63742,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -74634,7 +74634,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated the results and the report
</commit_message>
<xml_diff>
--- a/TP3/Results.xlsx
+++ b/TP3/Results.xlsx
@@ -233,7 +233,7 @@
   <dimension ref="A1:O559"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26532,7 +26532,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="0" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -52847,7 +52847,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -63742,7 +63742,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -74634,7 +74634,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>